<commit_message>
Add function to change the menu V1
</commit_message>
<xml_diff>
--- a/Diagramme/SmartClock_Gantt-Diagramm_V2.xlsx
+++ b/Diagramme/SmartClock_Gantt-Diagramm_V2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="514" documentId="8_{0C4EAEB1-A5C4-4402-980F-B32D81185735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E649FE74-D660-49D8-895C-A19D8947CDAA}"/>
+  <xr:revisionPtr revIDLastSave="527" documentId="8_{0C4EAEB1-A5C4-4402-980F-B32D81185735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BCAD768-584A-4D29-82E7-D778B1CF5DB1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1259,34 +1259,23 @@
     <cellStyle name="Überschrift 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="zAusgeblText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="115">
+  <dxfs count="81">
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
       <border>
         <left/>
         <right/>
         <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1359,338 +1348,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1709,36 +1366,40 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border>
         <left/>
         <right/>
         <top/>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
       <border>
         <left/>
         <right/>
         <top/>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2365,148 +2026,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2852,21 +2371,21 @@
   </dxfs>
   <tableStyles count="2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt-Tabellenformat" pivot="0" count="4" xr9:uid="{4904D139-63E4-4221-B7C9-C6C5B7A50FAF}">
-      <tableStyleElement type="wholeTable" dxfId="114"/>
-      <tableStyleElement type="headerRow" dxfId="113"/>
-      <tableStyleElement type="firstRowStripe" dxfId="112"/>
-      <tableStyleElement type="secondRowStripe" dxfId="111"/>
+      <tableStyleElement type="wholeTable" dxfId="80"/>
+      <tableStyleElement type="headerRow" dxfId="79"/>
+      <tableStyleElement type="firstRowStripe" dxfId="78"/>
+      <tableStyleElement type="secondRowStripe" dxfId="77"/>
     </tableStyle>
     <tableStyle name="Aufgabenliste" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="110"/>
-      <tableStyleElement type="headerRow" dxfId="109"/>
-      <tableStyleElement type="totalRow" dxfId="108"/>
-      <tableStyleElement type="firstColumn" dxfId="107"/>
-      <tableStyleElement type="lastColumn" dxfId="106"/>
-      <tableStyleElement type="firstRowStripe" dxfId="105"/>
-      <tableStyleElement type="secondRowStripe" dxfId="104"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="103"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="102"/>
+      <tableStyleElement type="wholeTable" dxfId="76"/>
+      <tableStyleElement type="headerRow" dxfId="75"/>
+      <tableStyleElement type="totalRow" dxfId="74"/>
+      <tableStyleElement type="firstColumn" dxfId="73"/>
+      <tableStyleElement type="lastColumn" dxfId="72"/>
+      <tableStyleElement type="firstRowStripe" dxfId="71"/>
+      <tableStyleElement type="secondRowStripe" dxfId="70"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="69"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="68"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3018,7 +2537,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Meilensteine4352" displayName="Meilensteine4352" ref="B9:G36" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Meilensteine4352" displayName="Meilensteine4352" ref="B9:G36" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="B9:G36" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3028,12 +2547,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Meilensteinbeschreibung" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Kategorie" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Zeitaufwand in std" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Fortschritt" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="95" dataCellStyle="Datum"/>
-    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Tage" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Meilensteinbeschreibung" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Kategorie" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Zeitaufwand in std" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Fortschritt" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="61" dataCellStyle="Datum"/>
+    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Tage" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="Aufgabenliste" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3045,7 +2564,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Meilensteine435" displayName="Meilensteine435" ref="B9:G36" totalsRowShown="0" headerRowDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Meilensteine435" displayName="Meilensteine435" ref="B9:G36" totalsRowShown="0" headerRowDxfId="59">
   <autoFilter ref="B9:G36" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3055,9 +2574,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Meilensteinbeschreibung" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Kategorie" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="   " dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Meilensteinbeschreibung" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Kategorie" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="   " dataDxfId="56"/>
     <tableColumn id="4" xr3:uid="{62B00BEF-16BE-4692-B5E2-F287F680F2C1}" name="Fortschritt"/>
     <tableColumn id="5" xr3:uid="{D6D72902-F68F-4E59-A714-AFFF520C647A}" name="Start" dataCellStyle="Datum"/>
     <tableColumn id="6" xr3:uid="{93E698DE-286F-49ED-AA20-D0C843671DE8}" name="Tage"/>
@@ -3072,7 +2591,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876EA49D-634E-482B-8173-880F7B761E2C}" name="Meilensteine43524" displayName="Meilensteine43524" ref="B9:G36" totalsRowShown="0" headerRowDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876EA49D-634E-482B-8173-880F7B761E2C}" name="Meilensteine43524" displayName="Meilensteine43524" ref="B9:G36" totalsRowShown="0" headerRowDxfId="55">
   <autoFilter ref="B9:G36" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3082,9 +2601,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0971B905-713A-4980-8BBC-DF959C2E61F9}" name="Meilensteinbeschreibung" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{4492A0B8-068F-4002-9E8D-E1F5FED367F0}" name="Kategorie" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{DF1A764E-7050-4528-B7F9-B6AB99372146}" name="Zugewiesen zu" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{0971B905-713A-4980-8BBC-DF959C2E61F9}" name="Meilensteinbeschreibung" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{4492A0B8-068F-4002-9E8D-E1F5FED367F0}" name="Kategorie" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{DF1A764E-7050-4528-B7F9-B6AB99372146}" name="Zugewiesen zu" dataDxfId="52"/>
     <tableColumn id="4" xr3:uid="{47C54592-75B0-4C70-BBF8-0F40483670E9}" name="Fortschritt"/>
     <tableColumn id="5" xr3:uid="{663FB5E0-7616-4EA5-B56A-FF069E2E07D7}" name="Start" dataCellStyle="Datum"/>
     <tableColumn id="6" xr3:uid="{3B766962-C06F-4E12-BE91-12AB93439874}" name="Tage"/>
@@ -10476,39 +9995,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="85" priority="4">
+    <cfRule type="expression" dxfId="51" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="84" priority="2">
+    <cfRule type="expression" dxfId="50" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="83" priority="1">
+    <cfRule type="expression" dxfId="49" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="82" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="7" stopIfTrue="1">
       <formula>AND($C10="Geringes Risiko",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="8" stopIfTrue="1">
       <formula>AND($C10="Hohes Risiko",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="9" stopIfTrue="1">
       <formula>AND($C10="Im Plan",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="10" stopIfTrue="1">
       <formula>AND($C10="Mittleres Risiko",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="77" priority="3">
+    <cfRule type="expression" dxfId="43" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10608,8 +10127,8 @@
   </sheetPr>
   <dimension ref="A1:BP38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AM13" sqref="AM13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C9" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AI19" sqref="AI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10920,9 +10439,8 @@
       <c r="B6" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="33" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Meilensteine435[Start])=0,TODAY(),B11(Meilensteine435[Start])),TODAY())</f>
-        <v>45965</v>
+      <c r="C6" s="33">
+        <v>45964</v>
       </c>
       <c r="D6" s="52"/>
       <c r="E6" s="31"/>
@@ -11026,227 +10544,227 @@
       <c r="H7" s="28"/>
       <c r="I7" s="95">
         <f ca="1">IFERROR(Projekt_Start+Scrollschrittweite,TODAY())</f>
-        <v>45966</v>
+        <v>45965</v>
       </c>
       <c r="J7" s="17">
         <f ca="1">I7+1</f>
-        <v>45967</v>
+        <v>45966</v>
       </c>
       <c r="K7" s="17">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45968</v>
+        <v>45967</v>
       </c>
       <c r="L7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45969</v>
+        <v>45968</v>
       </c>
       <c r="M7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="N7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45971</v>
+        <v>45970</v>
       </c>
       <c r="O7" s="63">
         <f t="shared" ca="1" si="0"/>
-        <v>45972</v>
+        <v>45971</v>
       </c>
       <c r="P7" s="17">
         <f ca="1">O7+1</f>
-        <v>45973</v>
+        <v>45972</v>
       </c>
       <c r="Q7" s="17">
         <f ca="1">P7+1</f>
-        <v>45974</v>
+        <v>45973</v>
       </c>
       <c r="R7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45975</v>
+        <v>45974</v>
       </c>
       <c r="S7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="T7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45977</v>
+        <v>45976</v>
       </c>
       <c r="U7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45978</v>
+        <v>45977</v>
       </c>
       <c r="V7" s="63">
         <f t="shared" ca="1" si="0"/>
-        <v>45979</v>
+        <v>45978</v>
       </c>
       <c r="W7" s="17">
         <f ca="1">V7+1</f>
-        <v>45980</v>
+        <v>45979</v>
       </c>
       <c r="X7" s="17">
         <f ca="1">W7+1</f>
-        <v>45981</v>
+        <v>45980</v>
       </c>
       <c r="Y7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45982</v>
+        <v>45981</v>
       </c>
       <c r="Z7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45983</v>
+        <v>45982</v>
       </c>
       <c r="AA7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45984</v>
+        <v>45983</v>
       </c>
       <c r="AB7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45985</v>
+        <v>45984</v>
       </c>
       <c r="AC7" s="63">
         <f t="shared" ca="1" si="0"/>
-        <v>45986</v>
+        <v>45985</v>
       </c>
       <c r="AD7" s="17">
         <f ca="1">AC7+1</f>
-        <v>45987</v>
+        <v>45986</v>
       </c>
       <c r="AE7" s="17">
         <f ca="1">AD7+1</f>
-        <v>45988</v>
+        <v>45987</v>
       </c>
       <c r="AF7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45989</v>
+        <v>45988</v>
       </c>
       <c r="AG7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45990</v>
+        <v>45989</v>
       </c>
       <c r="AH7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45991</v>
+        <v>45990</v>
       </c>
       <c r="AI7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45992</v>
+        <v>45991</v>
       </c>
       <c r="AJ7" s="63">
         <f t="shared" ca="1" si="0"/>
-        <v>45993</v>
+        <v>45992</v>
       </c>
       <c r="AK7" s="17">
         <f ca="1">AJ7+1</f>
-        <v>45994</v>
+        <v>45993</v>
       </c>
       <c r="AL7" s="17">
         <f ca="1">AK7+1</f>
-        <v>45995</v>
+        <v>45994</v>
       </c>
       <c r="AM7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45996</v>
+        <v>45995</v>
       </c>
       <c r="AN7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45997</v>
+        <v>45996</v>
       </c>
       <c r="AO7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45998</v>
+        <v>45997</v>
       </c>
       <c r="AP7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45999</v>
+        <v>45998</v>
       </c>
       <c r="AQ7" s="63">
         <f t="shared" ca="1" si="0"/>
-        <v>46000</v>
+        <v>45999</v>
       </c>
       <c r="AR7" s="17">
         <f ca="1">AQ7+1</f>
-        <v>46001</v>
+        <v>46000</v>
       </c>
       <c r="AS7" s="17">
         <f ca="1">AR7+1</f>
-        <v>46002</v>
+        <v>46001</v>
       </c>
       <c r="AT7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>46003</v>
+        <v>46002</v>
       </c>
       <c r="AU7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>46004</v>
+        <v>46003</v>
       </c>
       <c r="AV7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>46005</v>
+        <v>46004</v>
       </c>
       <c r="AW7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>46006</v>
+        <v>46005</v>
       </c>
       <c r="AX7" s="63">
         <f t="shared" ca="1" si="0"/>
-        <v>46007</v>
+        <v>46006</v>
       </c>
       <c r="AY7" s="17">
         <f ca="1">AX7+1</f>
-        <v>46008</v>
+        <v>46007</v>
       </c>
       <c r="AZ7" s="17">
         <f ca="1">AY7+1</f>
-        <v>46009</v>
+        <v>46008</v>
       </c>
       <c r="BA7" s="17">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>46010</v>
+        <v>46009</v>
       </c>
       <c r="BB7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>46011</v>
+        <v>46010</v>
       </c>
       <c r="BC7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>46012</v>
+        <v>46011</v>
       </c>
       <c r="BD7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>46013</v>
+        <v>46012</v>
       </c>
       <c r="BE7" s="63">
         <f t="shared" ca="1" si="1"/>
-        <v>46014</v>
+        <v>46013</v>
       </c>
       <c r="BF7" s="17">
         <f ca="1">BE7+1</f>
-        <v>46015</v>
+        <v>46014</v>
       </c>
       <c r="BG7" s="17">
         <f ca="1">BF7+1</f>
-        <v>46016</v>
+        <v>46015</v>
       </c>
       <c r="BH7" s="17">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>46017</v>
+        <v>46016</v>
       </c>
       <c r="BI7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>46018</v>
+        <v>46017</v>
       </c>
       <c r="BJ7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>46019</v>
+        <v>46018</v>
       </c>
       <c r="BK7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>46020</v>
+        <v>46019</v>
       </c>
       <c r="BL7" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>46021</v>
+        <v>46020</v>
       </c>
       <c r="BM7" s="31"/>
     </row>
@@ -11342,19 +10860,19 @@
       <c r="H9" s="47"/>
       <c r="I9" s="36" t="str">
         <f t="shared" ref="I9:AN9" ca="1" si="3">LEFT(TEXT(I7,"TTT"),1)</f>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="J9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="K9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="L9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="M9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11362,27 +10880,27 @@
       </c>
       <c r="N9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="O9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="P9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="Q9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="R9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="S9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="T9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11390,27 +10908,27 @@
       </c>
       <c r="U9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="V9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="W9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="X9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="Y9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="Z9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AA9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11418,27 +10936,27 @@
       </c>
       <c r="AB9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AC9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AD9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AE9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AF9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="AG9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AH9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11446,27 +10964,27 @@
       </c>
       <c r="AI9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AJ9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AK9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AL9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AM9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="AN9" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AO9" s="36" t="str">
         <f t="shared" ref="AO9:BL9" ca="1" si="4">LEFT(TEXT(AO7,"TTT"),1)</f>
@@ -11474,27 +10992,27 @@
       </c>
       <c r="AP9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AQ9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AR9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AS9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AT9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="AU9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AV9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -11502,27 +11020,27 @@
       </c>
       <c r="AW9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AX9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="AY9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AZ9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="BA9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="BB9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BC9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -11530,27 +11048,27 @@
       </c>
       <c r="BD9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BE9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="BF9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="BG9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="BH9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="BI9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BJ9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -11558,11 +11076,11 @@
       </c>
       <c r="BK9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BL9" s="36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>M</v>
       </c>
       <c r="BM9" s="31"/>
     </row>
@@ -12128,7 +11646,9 @@
       <c r="F13" s="23">
         <v>45965</v>
       </c>
-      <c r="G13" s="24"/>
+      <c r="G13" s="24">
+        <v>1</v>
+      </c>
       <c r="H13" s="19"/>
       <c r="I13" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -16005,7 +15525,7 @@
       <c r="G29" s="24"/>
       <c r="H29" s="19"/>
       <c r="I29" s="46" t="str">
-        <f t="shared" ref="I27:R35" ca="1" si="21">IF(AND($C29="Ziel",I$7&gt;=$F29,I$7&lt;=$F29+$G29-1),2,IF(AND($C29="Meilenstein",I$7&gt;=$F29,I$7&lt;=$F29+$G29-1),1,""))</f>
+        <f t="shared" ref="I29:R35" ca="1" si="21">IF(AND($C29="Ziel",I$7&gt;=$F29,I$7&lt;=$F29+$G29-1),2,IF(AND($C29="Meilenstein",I$7&gt;=$F29,I$7&lt;=$F29+$G29-1),1,""))</f>
         <v/>
       </c>
       <c r="J29" s="26" t="str">
@@ -16045,7 +15565,7 @@
         <v/>
       </c>
       <c r="S29" s="26" t="str">
-        <f t="shared" ref="S27:AB35" ca="1" si="22">IF(AND($C29="Ziel",S$7&gt;=$F29,S$7&lt;=$F29+$G29-1),2,IF(AND($C29="Meilenstein",S$7&gt;=$F29,S$7&lt;=$F29+$G29-1),1,""))</f>
+        <f t="shared" ref="S29:AB35" ca="1" si="22">IF(AND($C29="Ziel",S$7&gt;=$F29,S$7&lt;=$F29+$G29-1),2,IF(AND($C29="Meilenstein",S$7&gt;=$F29,S$7&lt;=$F29+$G29-1),1,""))</f>
         <v/>
       </c>
       <c r="T29" s="26" t="str">
@@ -16085,7 +15605,7 @@
         <v/>
       </c>
       <c r="AC29" s="26" t="str">
-        <f t="shared" ref="AC27:AL35" ca="1" si="23">IF(AND($C29="Ziel",AC$7&gt;=$F29,AC$7&lt;=$F29+$G29-1),2,IF(AND($C29="Meilenstein",AC$7&gt;=$F29,AC$7&lt;=$F29+$G29-1),1,""))</f>
+        <f t="shared" ref="AC29:AL35" ca="1" si="23">IF(AND($C29="Ziel",AC$7&gt;=$F29,AC$7&lt;=$F29+$G29-1),2,IF(AND($C29="Meilenstein",AC$7&gt;=$F29,AC$7&lt;=$F29+$G29-1),1,""))</f>
         <v/>
       </c>
       <c r="AD29" s="26" t="str">
@@ -16125,7 +15645,7 @@
         <v/>
       </c>
       <c r="AM29" s="26" t="str">
-        <f t="shared" ref="AM27:AV35" ca="1" si="24">IF(AND($C29="Ziel",AM$7&gt;=$F29,AM$7&lt;=$F29+$G29-1),2,IF(AND($C29="Meilenstein",AM$7&gt;=$F29,AM$7&lt;=$F29+$G29-1),1,""))</f>
+        <f t="shared" ref="AM29:AV35" ca="1" si="24">IF(AND($C29="Ziel",AM$7&gt;=$F29,AM$7&lt;=$F29+$G29-1),2,IF(AND($C29="Meilenstein",AM$7&gt;=$F29,AM$7&lt;=$F29+$G29-1),1,""))</f>
         <v/>
       </c>
       <c r="AN29" s="26" t="str">
@@ -17756,124 +17276,124 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="33" priority="4">
+    <cfRule type="expression" dxfId="42" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="32" priority="2">
+    <cfRule type="expression" dxfId="41" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="31" priority="1">
+    <cfRule type="expression" dxfId="40" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL16 I12:BK25 I23:BB28">
-    <cfRule type="expression" dxfId="0" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="7" stopIfTrue="1">
       <formula>AND($C10="Ist",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="8" stopIfTrue="1">
       <formula>AND($C10="Hohes Risiko",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="9" stopIfTrue="1">
       <formula>AND($C10="Soll",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="10" stopIfTrue="1">
       <formula>AND($C10="Mittleres Risiko",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:BL17">
-    <cfRule type="expression" dxfId="26" priority="411" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="411" stopIfTrue="1">
       <formula>AND($C19="Mittleres Risiko",I$7&gt;=$F19,I$7&lt;=$F19+$G19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="410" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="410" stopIfTrue="1">
       <formula>AND($C19="Im Plan",I$7&gt;=$F19,I$7&lt;=$F19+$G19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="409" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="409" stopIfTrue="1">
       <formula>AND($C19="Hohes Risiko",I$7&gt;=$F19,I$7&lt;=$F19+$G19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="408" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="408" stopIfTrue="1">
       <formula>AND($C19="Geringes Risiko",I$7&gt;=$F19,I$7&lt;=$F19+$G19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="412" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="412" stopIfTrue="1">
       <formula>AND(LEN($C19)=0,I$7&gt;=$F19,I$7&lt;=$F19+$G19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:BL19">
-    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="36" stopIfTrue="1">
       <formula>AND($C17="Geringes Risiko",I$7&gt;=$F17,I$7&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="37" stopIfTrue="1">
       <formula>AND($C17="Hohes Risiko",I$7&gt;=$F17,I$7&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="38" stopIfTrue="1">
       <formula>AND($C17="Im Plan",I$7&gt;=$F17,I$7&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="39" stopIfTrue="1">
       <formula>AND($C17="Mittleres Risiko",I$7&gt;=$F17,I$7&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="40" stopIfTrue="1">
       <formula>AND(LEN($C17)=0,I$7&gt;=$F17,I$7&lt;=$F17+$G17-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:BL23 I23:BB28">
-    <cfRule type="expression" dxfId="16" priority="402" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="402" stopIfTrue="1">
       <formula>AND($C20="Geringes Risiko",I$7&gt;=$F20,I$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="404" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="404" stopIfTrue="1">
       <formula>AND($C20="Im Plan",I$7&gt;=$F20,I$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="405" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="405" stopIfTrue="1">
       <formula>AND($C20="Mittleres Risiko",I$7&gt;=$F20,I$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="406" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="406" stopIfTrue="1">
       <formula>AND(LEN($C20)=0,I$7&gt;=$F20,I$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="403" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="403" stopIfTrue="1">
       <formula>AND($C20="Hohes Risiko",I$7&gt;=$F20,I$7&lt;=$F20+$G20-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:BL24">
-    <cfRule type="expression" dxfId="11" priority="368" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="368" stopIfTrue="1">
       <formula>AND(LEN($C24)=0,I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="366" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="366" stopIfTrue="1">
       <formula>AND($C24="Im Plan",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="365" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="365" stopIfTrue="1">
       <formula>AND($C24="Hohes Risiko",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="364" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="364" stopIfTrue="1">
       <formula>AND($C24="Geringes Risiko",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="367" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="367" stopIfTrue="1">
       <formula>AND($C24="Mittleres Risiko",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25:BL35">
-    <cfRule type="expression" dxfId="6" priority="414" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="414" stopIfTrue="1">
       <formula>AND($C25="Geringes Risiko",I$7&gt;=$F25,I$7&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="415" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="415" stopIfTrue="1">
       <formula>AND($C25="Hohes Risiko",I$7&gt;=$F25,I$7&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="416" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="416" stopIfTrue="1">
       <formula>AND($C25="Im Plan",I$7&gt;=$F25,I$7&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="417" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="417" stopIfTrue="1">
       <formula>AND($C25="Mittleres Risiko",I$7&gt;=$F25,I$7&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="418" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="418" stopIfTrue="1">
       <formula>AND(LEN($C25)=0,I$7&gt;=$F25,I$7&lt;=$F25+$G25-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25086,39 +24606,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="76" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="75" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="74" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="73" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>AND($C10="Geringes Risiko",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
       <formula>AND($C10="Hohes Risiko",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
       <formula>AND($C10="Im Plan",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="10" stopIfTrue="1">
       <formula>AND($C10="Mittleres Risiko",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="68" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25215,12 +24735,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25518,29 +25049,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD6AD73-D703-40CF-AB8D-72E6A3921BEB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25567,13 +25091,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD6AD73-D703-40CF-AB8D-72E6A3921BEB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Delete unused sensor files and document additions to the project
</commit_message>
<xml_diff>
--- a/Diagramme/SmartClock_Gantt-Diagramm_V2.xlsx
+++ b/Diagramme/SmartClock_Gantt-Diagramm_V2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="532" documentId="8_{0C4EAEB1-A5C4-4402-980F-B32D81185735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A1A49F4-C99E-465C-8FA4-F2D000359528}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="8_{0C4EAEB1-A5C4-4402-980F-B32D81185735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{475EDA19-C605-435D-9E5F-DF4F5F9A0A6D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="57">
   <si>
     <t>INFORMATIONEN ZU DIESEM GANTT-DIAGRAMM</t>
   </si>
@@ -184,9 +184,6 @@
 Alle Projektzeitplandiagramme werden automatisch generiert.</t>
   </si>
   <si>
-    <t xml:space="preserve">   </t>
-  </si>
-  <si>
     <t>SmartClock</t>
   </si>
   <si>
@@ -233,6 +230,21 @@
   </si>
   <si>
     <t>Evaluate</t>
+  </si>
+  <si>
+    <t>Aufwand Soll / Ist</t>
+  </si>
+  <si>
+    <t>14h</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>4.5h</t>
+  </si>
+  <si>
+    <t>16h</t>
   </si>
 </sst>
 </file>
@@ -2576,7 +2588,7 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Meilensteinbeschreibung" dataDxfId="58"/>
     <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Kategorie" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="   " dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Aufwand Soll / Ist" dataDxfId="56"/>
     <tableColumn id="4" xr3:uid="{62B00BEF-16BE-4692-B5E2-F287F680F2C1}" name="Fortschritt"/>
     <tableColumn id="5" xr3:uid="{D6D72902-F68F-4E59-A714-AFFF520C647A}" name="Start" dataCellStyle="Datum"/>
     <tableColumn id="6" xr3:uid="{93E698DE-286F-49ED-AA20-D0C843671DE8}" name="Tage"/>
@@ -3077,7 +3089,7 @@
     <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="130" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="130"/>
       <c r="D2" s="130"/>
@@ -3160,7 +3172,7 @@
     <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="72"/>
       <c r="D4" s="73"/>
@@ -3208,7 +3220,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="77" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="73"/>
       <c r="D5" s="73"/>
@@ -3626,7 +3638,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="125" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="114" t="s">
         <v>28</v>
@@ -3930,10 +3942,10 @@
     <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="126" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="58"/>
       <c r="E11" s="59">
@@ -4176,7 +4188,7 @@
       <c r="A12" s="10"/>
       <c r="B12" s="126"/>
       <c r="C12" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="58"/>
       <c r="E12" s="59">
@@ -4417,10 +4429,10 @@
     <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="126" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="58"/>
       <c r="E13" s="59">
@@ -4662,7 +4674,7 @@
       <c r="A14" s="9"/>
       <c r="B14" s="126"/>
       <c r="C14" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="58"/>
       <c r="E14" s="59">
@@ -4903,10 +4915,10 @@
     <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="126" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="58"/>
       <c r="E15" s="59">
@@ -5148,7 +5160,7 @@
       <c r="A16" s="9"/>
       <c r="B16" s="126"/>
       <c r="C16" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="58"/>
       <c r="E16" s="59">
@@ -5389,10 +5401,10 @@
     <row r="17" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="126" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="58"/>
       <c r="E17" s="59">
@@ -5634,7 +5646,7 @@
       <c r="A18" s="10"/>
       <c r="B18" s="126"/>
       <c r="C18" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="58"/>
       <c r="E18" s="59">
@@ -5875,10 +5887,10 @@
     <row r="19" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="126" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="58"/>
       <c r="E19" s="59">
@@ -6120,7 +6132,7 @@
       <c r="A20" s="9"/>
       <c r="B20" s="126"/>
       <c r="C20" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="58"/>
       <c r="E20" s="59">
@@ -6361,10 +6373,10 @@
     <row r="21" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="126" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="58"/>
       <c r="E21" s="59">
@@ -6606,7 +6618,7 @@
       <c r="A22" s="9"/>
       <c r="B22" s="126"/>
       <c r="C22" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="58"/>
       <c r="E22" s="59">
@@ -6847,7 +6859,7 @@
     <row r="23" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="126" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="58"/>
       <c r="D23" s="58"/>
@@ -7317,7 +7329,7 @@
     <row r="25" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="126" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="58"/>
       <c r="D25" s="58"/>
@@ -7787,7 +7799,7 @@
     <row r="27" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="126" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="58"/>
       <c r="D27" s="58"/>
@@ -10127,8 +10139,8 @@
   </sheetPr>
   <dimension ref="A1:BP38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A9" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y12:Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10285,7 +10297,7 @@
     <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="50"/>
@@ -10296,7 +10308,7 @@
       </c>
       <c r="H4" s="28"/>
       <c r="I4" s="133" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" s="133"/>
       <c r="K4" s="133"/>
@@ -10305,7 +10317,7 @@
       <c r="N4" s="133"/>
       <c r="O4" s="31"/>
       <c r="P4" s="140" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q4" s="140"/>
       <c r="R4" s="140"/>
@@ -10368,7 +10380,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="51"/>
@@ -10846,7 +10858,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="119" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E9" s="119" t="s">
         <v>28</v>
@@ -11153,7 +11165,7 @@
     <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="122" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -11391,12 +11403,14 @@
     <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="123" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="21"/>
+        <v>41</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="E12" s="22">
         <v>1</v>
       </c>
@@ -11637,9 +11651,11 @@
       <c r="A13" s="10"/>
       <c r="B13" s="123"/>
       <c r="C13" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="21"/>
+        <v>42</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E13" s="22">
         <v>1</v>
       </c>
@@ -11879,12 +11895,14 @@
     <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="123" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="21"/>
+        <v>41</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="E14" s="22">
         <v>0.5</v>
       </c>
@@ -12125,16 +12143,20 @@
       <c r="A15" s="9"/>
       <c r="B15" s="123"/>
       <c r="C15" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="21"/>
+        <v>42</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>56</v>
+      </c>
       <c r="E15" s="22">
         <v>0.5</v>
       </c>
       <c r="F15" s="23">
-        <v>45967</v>
-      </c>
-      <c r="G15" s="24"/>
+        <v>45966</v>
+      </c>
+      <c r="G15" s="24">
+        <v>9</v>
+      </c>
       <c r="H15" s="19"/>
       <c r="I15" s="46" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -12365,12 +12387,14 @@
     <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="123" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="21"/>
+        <v>41</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="E16" s="22">
         <v>0</v>
       </c>
@@ -12378,7 +12402,7 @@
         <v>45972</v>
       </c>
       <c r="G16" s="24">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="46" t="str">
@@ -12611,16 +12635,18 @@
       <c r="A17" s="10"/>
       <c r="B17" s="123"/>
       <c r="C17" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="22">
         <v>0</v>
       </c>
       <c r="F17" s="23">
-        <v>45972</v>
-      </c>
-      <c r="G17" s="24"/>
+        <v>45974</v>
+      </c>
+      <c r="G17" s="24">
+        <v>1</v>
+      </c>
       <c r="H17" s="19"/>
       <c r="I17" s="46" t="str">
         <f t="shared" ref="I17:X28" ca="1" si="14">IF(AND($C17="Ziel",I$7&gt;=$F17,I$7&lt;=$F17+$G17-1),2,IF(AND($C17="Meilenstein",I$7&gt;=$F17,I$7&lt;=$F17+$G17-1),1,""))</f>
@@ -12851,10 +12877,10 @@
     <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="123" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="22">
@@ -13097,7 +13123,7 @@
       <c r="A19" s="9"/>
       <c r="B19" s="123"/>
       <c r="C19" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="22">
@@ -13337,10 +13363,10 @@
     <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="123" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22">
@@ -13583,7 +13609,7 @@
       <c r="A21" s="9"/>
       <c r="B21" s="123"/>
       <c r="C21" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="22">
@@ -13823,10 +13849,10 @@
     <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="123" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="22">
@@ -14069,7 +14095,7 @@
       <c r="A23" s="9"/>
       <c r="B23" s="123"/>
       <c r="C23" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="22">
@@ -14309,10 +14335,10 @@
     <row r="24" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="123" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="22">
@@ -14555,7 +14581,7 @@
       <c r="A25" s="9"/>
       <c r="B25" s="123"/>
       <c r="C25" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="22">
@@ -14795,10 +14821,10 @@
     <row r="26" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="123" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="22">
@@ -15041,7 +15067,7 @@
       <c r="A27" s="9"/>
       <c r="B27" s="123"/>
       <c r="C27" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
@@ -15280,7 +15306,7 @@
       <c r="A28" s="9"/>
       <c r="B28" s="123"/>
       <c r="C28" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
@@ -15517,7 +15543,7 @@
       <c r="A29" s="9"/>
       <c r="B29" s="124"/>
       <c r="C29" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
@@ -15754,7 +15780,7 @@
       <c r="A30" s="9"/>
       <c r="B30" s="123"/>
       <c r="C30" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
@@ -15991,7 +16017,7 @@
       <c r="A31" s="9"/>
       <c r="B31" s="123"/>
       <c r="C31" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
@@ -16228,7 +16254,7 @@
       <c r="A32" s="9"/>
       <c r="B32" s="123"/>
       <c r="C32" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
@@ -16465,7 +16491,7 @@
       <c r="A33" s="9"/>
       <c r="B33" s="123"/>
       <c r="C33" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
@@ -16702,7 +16728,7 @@
       <c r="A34" s="9"/>
       <c r="B34" s="123"/>
       <c r="C34" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
@@ -16939,7 +16965,7 @@
       <c r="A35" s="9"/>
       <c r="B35" s="123"/>
       <c r="C35" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
@@ -17766,7 +17792,7 @@
       </c>
       <c r="C6" s="79" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Meilensteine43524[Start])=0,TODAY(),B11(Meilensteine43524[Start])),TODAY())</f>
-        <v>45972</v>
+        <v>45974</v>
       </c>
       <c r="D6" s="80"/>
       <c r="E6" s="74"/>
@@ -17845,7 +17871,7 @@
       <c r="BE6" s="89"/>
       <c r="BF6" s="89" t="str">
         <f ca="1">IF(OR(TEXT(BF7,"MMMM")=AY6,TEXT(BF7,"MMMM")=AR6,TEXT(BF7,"MMMM")=AK6,TEXT(BF7,"MMMM")=AD6),"",TEXT(BF7,"MMMM"))</f>
-        <v/>
+        <v>Januar</v>
       </c>
       <c r="BG6" s="89"/>
       <c r="BH6" s="89"/>
@@ -17869,227 +17895,227 @@
       <c r="H7" s="82"/>
       <c r="I7" s="97">
         <f ca="1">IFERROR(Projekt_Start+Scrollschrittweite,TODAY())</f>
-        <v>45973</v>
+        <v>45975</v>
       </c>
       <c r="J7" s="98">
         <f ca="1">I7+1</f>
-        <v>45974</v>
+        <v>45976</v>
       </c>
       <c r="K7" s="98">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45975</v>
+        <v>45977</v>
       </c>
       <c r="L7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45976</v>
+        <v>45978</v>
       </c>
       <c r="M7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45977</v>
+        <v>45979</v>
       </c>
       <c r="N7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45978</v>
+        <v>45980</v>
       </c>
       <c r="O7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45979</v>
+        <v>45981</v>
       </c>
       <c r="P7" s="98">
         <f ca="1">O7+1</f>
-        <v>45980</v>
+        <v>45982</v>
       </c>
       <c r="Q7" s="98">
         <f ca="1">P7+1</f>
-        <v>45981</v>
+        <v>45983</v>
       </c>
       <c r="R7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45982</v>
+        <v>45984</v>
       </c>
       <c r="S7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45983</v>
+        <v>45985</v>
       </c>
       <c r="T7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45984</v>
+        <v>45986</v>
       </c>
       <c r="U7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45985</v>
+        <v>45987</v>
       </c>
       <c r="V7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45986</v>
+        <v>45988</v>
       </c>
       <c r="W7" s="98">
         <f ca="1">V7+1</f>
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="X7" s="98">
         <f ca="1">W7+1</f>
-        <v>45988</v>
+        <v>45990</v>
       </c>
       <c r="Y7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45989</v>
+        <v>45991</v>
       </c>
       <c r="Z7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45990</v>
+        <v>45992</v>
       </c>
       <c r="AA7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="AB7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="AC7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="AD7" s="98">
         <f ca="1">AC7+1</f>
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="AE7" s="98">
         <f ca="1">AD7+1</f>
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="AF7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="AG7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="AH7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="AI7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="AJ7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="AK7" s="98">
         <f ca="1">AJ7+1</f>
-        <v>46001</v>
+        <v>46003</v>
       </c>
       <c r="AL7" s="98">
         <f ca="1">AK7+1</f>
-        <v>46002</v>
+        <v>46004</v>
       </c>
       <c r="AM7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>46003</v>
+        <v>46005</v>
       </c>
       <c r="AN7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>46004</v>
+        <v>46006</v>
       </c>
       <c r="AO7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>46005</v>
+        <v>46007</v>
       </c>
       <c r="AP7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>46006</v>
+        <v>46008</v>
       </c>
       <c r="AQ7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>46007</v>
+        <v>46009</v>
       </c>
       <c r="AR7" s="98">
         <f ca="1">AQ7+1</f>
-        <v>46008</v>
+        <v>46010</v>
       </c>
       <c r="AS7" s="98">
         <f ca="1">AR7+1</f>
-        <v>46009</v>
+        <v>46011</v>
       </c>
       <c r="AT7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>46010</v>
+        <v>46012</v>
       </c>
       <c r="AU7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>46011</v>
+        <v>46013</v>
       </c>
       <c r="AV7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>46012</v>
+        <v>46014</v>
       </c>
       <c r="AW7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>46013</v>
+        <v>46015</v>
       </c>
       <c r="AX7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>46014</v>
+        <v>46016</v>
       </c>
       <c r="AY7" s="98">
         <f ca="1">AX7+1</f>
-        <v>46015</v>
+        <v>46017</v>
       </c>
       <c r="AZ7" s="98">
         <f ca="1">AY7+1</f>
-        <v>46016</v>
+        <v>46018</v>
       </c>
       <c r="BA7" s="98">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>46017</v>
+        <v>46019</v>
       </c>
       <c r="BB7" s="98">
         <f t="shared" ca="1" si="1"/>
-        <v>46018</v>
+        <v>46020</v>
       </c>
       <c r="BC7" s="98">
         <f t="shared" ca="1" si="1"/>
-        <v>46019</v>
+        <v>46021</v>
       </c>
       <c r="BD7" s="98">
         <f t="shared" ca="1" si="1"/>
-        <v>46020</v>
+        <v>46022</v>
       </c>
       <c r="BE7" s="99">
         <f t="shared" ca="1" si="1"/>
-        <v>46021</v>
+        <v>46023</v>
       </c>
       <c r="BF7" s="98">
         <f ca="1">BE7+1</f>
-        <v>46022</v>
+        <v>46024</v>
       </c>
       <c r="BG7" s="98">
         <f ca="1">BF7+1</f>
-        <v>46023</v>
+        <v>46025</v>
       </c>
       <c r="BH7" s="98">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>46024</v>
+        <v>46026</v>
       </c>
       <c r="BI7" s="98">
         <f t="shared" ca="1" si="2"/>
-        <v>46025</v>
+        <v>46027</v>
       </c>
       <c r="BJ7" s="98">
         <f t="shared" ca="1" si="2"/>
-        <v>46026</v>
+        <v>46028</v>
       </c>
       <c r="BK7" s="98">
         <f t="shared" ca="1" si="2"/>
-        <v>46027</v>
+        <v>46029</v>
       </c>
       <c r="BL7" s="99">
         <f t="shared" ca="1" si="2"/>
-        <v>46028</v>
+        <v>46030</v>
       </c>
     </row>
     <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -18183,23 +18209,23 @@
       <c r="H9" s="87"/>
       <c r="I9" s="105" t="str">
         <f t="shared" ref="I9:AN9" ca="1" si="3">LEFT(TEXT(I7,"TTT"),1)</f>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="J9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="K9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="L9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="M9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="N9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18211,23 +18237,23 @@
       </c>
       <c r="P9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="Q9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="R9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="S9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="T9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="U9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18239,23 +18265,23 @@
       </c>
       <c r="W9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="X9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="Y9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="Z9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AA9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AB9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18267,23 +18293,23 @@
       </c>
       <c r="AD9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AE9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AF9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AG9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AH9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AI9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -18295,23 +18321,23 @@
       </c>
       <c r="AK9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AL9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AM9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AN9" s="105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AO9" s="105" t="str">
         <f t="shared" ref="AO9:BL9" ca="1" si="4">LEFT(TEXT(AO7,"TTT"),1)</f>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AP9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -18323,23 +18349,23 @@
       </c>
       <c r="AR9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AS9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AT9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AU9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AV9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AW9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -18351,23 +18377,23 @@
       </c>
       <c r="AY9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AZ9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BA9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="BB9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BC9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BD9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -18379,23 +18405,23 @@
       </c>
       <c r="BF9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="BG9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BH9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="BI9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BJ9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BK9" s="105" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -18723,7 +18749,7 @@
       </c>
       <c r="F12" s="60">
         <f ca="1">TODAY()</f>
-        <v>45972</v>
+        <v>45974</v>
       </c>
       <c r="G12" s="61">
         <v>3</v>
@@ -18966,7 +18992,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="60">
         <f ca="1">TODAY()+5</f>
-        <v>45977</v>
+        <v>45979</v>
       </c>
       <c r="G13" s="61">
         <v>1</v>
@@ -19211,7 +19237,7 @@
       </c>
       <c r="F14" s="60">
         <f ca="1">F12-3</f>
-        <v>45969</v>
+        <v>45971</v>
       </c>
       <c r="G14" s="61">
         <v>10</v>
@@ -19454,7 +19480,7 @@
       <c r="E15" s="59"/>
       <c r="F15" s="60">
         <f ca="1">F12+20</f>
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="G15" s="61">
         <v>1</v>
@@ -19699,7 +19725,7 @@
       </c>
       <c r="F16" s="60">
         <f ca="1">F12+6</f>
-        <v>45978</v>
+        <v>45980</v>
       </c>
       <c r="G16" s="61">
         <v>6</v>
@@ -20180,7 +20206,7 @@
       </c>
       <c r="F18" s="60">
         <f ca="1">F12+6</f>
-        <v>45978</v>
+        <v>45980</v>
       </c>
       <c r="G18" s="61">
         <v>13</v>
@@ -20425,7 +20451,7 @@
       </c>
       <c r="F19" s="60">
         <f ca="1">F18+2</f>
-        <v>45980</v>
+        <v>45982</v>
       </c>
       <c r="G19" s="61">
         <v>9</v>
@@ -20670,7 +20696,7 @@
       </c>
       <c r="F20" s="60">
         <f ca="1">F19+5</f>
-        <v>45985</v>
+        <v>45987</v>
       </c>
       <c r="G20" s="61">
         <v>11</v>
@@ -20913,7 +20939,7 @@
       <c r="E21" s="59"/>
       <c r="F21" s="60">
         <f ca="1">F20+2</f>
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="G21" s="61">
         <v>1</v>
@@ -21154,7 +21180,7 @@
       <c r="E22" s="59"/>
       <c r="F22" s="60">
         <f ca="1">F21+1</f>
-        <v>45988</v>
+        <v>45990</v>
       </c>
       <c r="G22" s="61">
         <v>24</v>
@@ -21633,7 +21659,7 @@
       <c r="E24" s="59"/>
       <c r="F24" s="60">
         <f ca="1">F12+15</f>
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="G24" s="61">
         <v>4</v>
@@ -21876,7 +21902,7 @@
       <c r="E25" s="59"/>
       <c r="F25" s="60">
         <f ca="1">F24+3</f>
-        <v>45990</v>
+        <v>45992</v>
       </c>
       <c r="G25" s="61">
         <v>14</v>
@@ -22119,7 +22145,7 @@
       <c r="E26" s="59"/>
       <c r="F26" s="60">
         <f ca="1">F25+15</f>
-        <v>46005</v>
+        <v>46007</v>
       </c>
       <c r="G26" s="61">
         <v>6</v>
@@ -22362,7 +22388,7 @@
       <c r="E27" s="59"/>
       <c r="F27" s="60">
         <f ca="1">F21+22</f>
-        <v>46009</v>
+        <v>46011</v>
       </c>
       <c r="G27" s="61">
         <v>3</v>
@@ -22605,7 +22631,7 @@
       <c r="E28" s="59"/>
       <c r="F28" s="60">
         <f ca="1">F16</f>
-        <v>45978</v>
+        <v>45980</v>
       </c>
       <c r="G28" s="61">
         <v>19</v>
@@ -23082,7 +23108,7 @@
       <c r="E30" s="59"/>
       <c r="F30" s="60">
         <f ca="1">F27+3</f>
-        <v>46012</v>
+        <v>46014</v>
       </c>
       <c r="G30" s="61">
         <v>15</v>
@@ -23323,7 +23349,7 @@
       <c r="E31" s="59"/>
       <c r="F31" s="60">
         <f ca="1">F30+14</f>
-        <v>46026</v>
+        <v>46028</v>
       </c>
       <c r="G31" s="61">
         <v>5</v>
@@ -23566,7 +23592,7 @@
       <c r="E32" s="59"/>
       <c r="F32" s="60">
         <f ca="1">F31+42</f>
-        <v>46068</v>
+        <v>46070</v>
       </c>
       <c r="G32" s="61">
         <v>1</v>
@@ -25029,15 +25055,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -25055,6 +25072,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25079,14 +25105,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD6AD73-D703-40CF-AB8D-72E6A3921BEB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -25096,4 +25114,12 @@
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>